<commit_message>
Added comparison "Optimization versus No optimization"
</commit_message>
<xml_diff>
--- a/showroom/pic32mx_prefetch_cache/presentation/excel.xlsx
+++ b/showroom/pic32mx_prefetch_cache/presentation/excel.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015"/>
+    <workbookView xWindow="120" yWindow="12" windowWidth="19032" windowHeight="12012"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Chart4 (5)" sheetId="16" r:id="rId2"/>
-    <sheet name="Chart4 (3)" sheetId="14" r:id="rId3"/>
-    <sheet name="Chart4 (2)" sheetId="13" r:id="rId4"/>
-    <sheet name="Chart4 (4)" sheetId="15" r:id="rId5"/>
-    <sheet name="Chart4" sheetId="7" r:id="rId6"/>
+    <sheet name="Chart1" sheetId="17" r:id="rId2"/>
+    <sheet name="Chart4 (5)" sheetId="16" r:id="rId3"/>
+    <sheet name="Chart4 (3)" sheetId="14" r:id="rId4"/>
+    <sheet name="Chart4 (2)" sheetId="13" r:id="rId5"/>
+    <sheet name="Chart4 (4)" sheetId="15" r:id="rId6"/>
+    <sheet name="Chart4" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>Program Flash, Data Flash, Loop</t>
   </si>
@@ -61,6 +62,21 @@
   </si>
   <si>
     <t xml:space="preserve">Zero wait state RAM  </t>
+  </si>
+  <si>
+    <t>Optimizations level 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    </t>
+  </si>
+  <si>
+    <t>No optimizations</t>
+  </si>
+  <si>
+    <t>Program Flash, Data Flash, Loop, No optimization</t>
+  </si>
+  <si>
+    <t>Program Flash, Data Flash, Loop, Optimization Level 1</t>
   </si>
 </sst>
 </file>
@@ -120,18 +136,21 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Sheet1!$B$23:$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Program Flash, Data Flash, Loop</c:v>
+                  <c:v>Program Flash, Data Flash, Loop, No optimization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Sheet1!$A$24:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -157,27 +176,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:f>Sheet1!$B$24:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>340040</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>170022</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>139513</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>66514</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42520</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42519</c:v>
+                  <c:v>1080071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>540039</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>351522</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>251029</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>234529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -188,18 +207,21 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Sheet1!$C$23:$C$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Program Flash, Data RAM, Loop</c:v>
+                  <c:v>Program Flash, Data Flash, Loop, Optimization Level 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Sheet1!$A$24:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -225,459 +247,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:f>Sheet1!$C$24:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>404040</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>202022</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>90514</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>58515</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>58515</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50514</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Program RAM, Data Flash, Loop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Default              </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Min flash wait states</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Flash prefetch       </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Flash program cache  </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Flash data cache     </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Zero wait state RAM  </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$3:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>117013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>85013</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>85013</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>85013</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>69017</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>34513</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Program RAM, Data RAM, Loop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Default              </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Min flash wait states</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Flash prefetch       </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Flash program cache  </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Flash data cache     </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Zero wait state RAM  </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$3:$E$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>101013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>101013</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>101013</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>101013</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>101013</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>58507</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Program Flash, Data Flash, Sequence</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Default              </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Min flash wait states</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Flash prefetch       </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Flash program cache  </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Flash data cache     </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Zero wait state RAM  </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$3:$F$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>300604</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>150304</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>111281</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>96528</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>70222</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>64022</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Program Flash, Data RAM, Sequence</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Default              </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Min flash wait states</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Flash prefetch       </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Flash program cache  </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Flash data cache     </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Zero wait state RAM  </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$3:$G$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>237100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>118552</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>68779</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68590</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>68590</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>56764</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Program RAM, Data Flash, Sequence</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Default              </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Min flash wait states</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Flash prefetch       </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Flash program cache  </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Flash data cache     </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Zero wait state RAM  </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$3:$H$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>114345</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>82345</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>82346</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>82346</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>62287</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43468</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Program RAM, Data RAM, Sequence</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Default              </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Min flash wait states</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Flash prefetch       </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Flash program cache  </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Flash data cache     </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Zero wait state RAM  </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$I$3:$I$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>66594</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>66594</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66595</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>66594</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>66594</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>51024</c:v>
+                  <c:v>340040</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>139513</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66514</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110338816"/>
-        <c:axId val="110340352"/>
+        <c:axId val="69452160"/>
+        <c:axId val="69453696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110338816"/>
+        <c:axId val="69452160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110340352"/>
+        <c:crossAx val="69453696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110340352"/>
+        <c:axId val="69453696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,7 +299,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110338816"/>
+        <c:crossAx val="69452160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -776,8 +390,144 @@
           </c:val>
         </c:ser>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Program Flash, Data RAM, Loop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Default              </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Min flash wait states</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flash prefetch       </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Flash program cache  </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Flash data cache     </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Zero wait state RAM  </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>404040</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>202022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58515</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58515</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50514</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Program RAM, Data Flash, Loop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Default              </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Min flash wait states</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flash prefetch       </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Flash program cache  </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Flash data cache     </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Zero wait state RAM  </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>117013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34513</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$E$2</c:f>
@@ -843,25 +593,297 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Program Flash, Data Flash, Sequence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Default              </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Min flash wait states</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flash prefetch       </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Flash program cache  </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Flash data cache     </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Zero wait state RAM  </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>300604</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150304</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111281</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96528</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Program Flash, Data RAM, Sequence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Default              </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Min flash wait states</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flash prefetch       </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Flash program cache  </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Flash data cache     </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Zero wait state RAM  </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>237100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118552</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68779</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68590</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68590</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56764</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Program RAM, Data Flash, Sequence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Default              </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Min flash wait states</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flash prefetch       </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Flash program cache  </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Flash data cache     </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Zero wait state RAM  </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>114345</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82345</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82346</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82346</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62287</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43468</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Program RAM, Data RAM, Sequence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Default              </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Min flash wait states</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flash prefetch       </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Flash program cache  </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Flash data cache     </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Zero wait state RAM  </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$3:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>66594</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66594</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66595</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66594</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66594</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101751808"/>
-        <c:axId val="101771904"/>
+        <c:axId val="50034176"/>
+        <c:axId val="50035712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101751808"/>
+        <c:axId val="50034176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101771904"/>
+        <c:crossAx val="50035712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101771904"/>
+        <c:axId val="50035712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,7 +891,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101751808"/>
+        <c:crossAx val="50034176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -892,15 +914,15 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Sheet1!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Program Flash, Data RAM, Loop</c:v>
+                  <c:v>Program Flash, Data Flash, Loop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -933,27 +955,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>404040</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>202022</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>90514</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>58515</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>58515</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50514</c:v>
+                  <c:v>340040</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>139513</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66514</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1028,24 +1050,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="73549696"/>
-        <c:axId val="73551232"/>
+        <c:axId val="49958272"/>
+        <c:axId val="49984640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73549696"/>
+        <c:axId val="49958272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73551232"/>
+        <c:crossAx val="49984640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73551232"/>
+        <c:axId val="49984640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,7 +1075,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73549696"/>
+        <c:crossAx val="49958272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1076,76 +1098,8 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Program Flash, Data Flash, Loop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Default              </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Min flash wait states</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Flash prefetch       </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Flash program cache  </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Flash data cache     </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Zero wait state RAM  </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>340040</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>170022</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>139513</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>66514</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42520</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42519</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$C$2</c:f>
@@ -1211,25 +1165,93 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Program RAM, Data RAM, Loop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Default              </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Min flash wait states</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flash prefetch       </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Flash program cache  </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Flash data cache     </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Zero wait state RAM  </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>101013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>101013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101013</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58507</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101973376"/>
-        <c:axId val="102044800"/>
+        <c:axId val="50079232"/>
+        <c:axId val="50080768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101973376"/>
+        <c:axId val="50079232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102044800"/>
+        <c:crossAx val="50080768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102044800"/>
+        <c:axId val="50080768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,7 +1259,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101973376"/>
+        <c:crossAx val="50079232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1328,15 +1350,15 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
+              <c:f>Sheet1!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Program Flash, Data Flash, Sequence</c:v>
+                  <c:v>Program Flash, Data RAM, Loop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1369,51 +1391,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$8</c:f>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>300604</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>150304</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>111281</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>96528</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>70222</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>64022</c:v>
+                  <c:v>404040</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>202022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58515</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58515</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50514</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84422656"/>
-        <c:axId val="84425344"/>
+        <c:axId val="50154880"/>
+        <c:axId val="50160768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84422656"/>
+        <c:axId val="50154880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84425344"/>
+        <c:crossAx val="50160768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84425344"/>
+        <c:axId val="50160768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1421,7 +1443,191 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84422656"/>
+        <c:crossAx val="50154880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Program Flash, Data Flash, Loop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Default              </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Min flash wait states</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flash prefetch       </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Flash program cache  </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Flash data cache     </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Zero wait state RAM  </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>340040</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>139513</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66514</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42519</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Program Flash, Data Flash, Sequence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Default              </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Min flash wait states</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Flash prefetch       </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Flash program cache  </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Flash data cache     </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Zero wait state RAM  </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>300604</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150304</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111281</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96528</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50202112"/>
+        <c:axId val="50203648"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50202112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50203648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50203648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50202112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1439,7 +1645,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1450,7 +1656,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1461,7 +1667,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1472,7 +1678,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1483,7 +1689,18 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1494,7 +1711,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670192" cy="6293013"/>
+    <xdr:ext cx="8661400" cy="6290733"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1599,6 +1816,33 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8670192" cy="6293013"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -1910,16 +2154,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I8"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="9" width="17.42578125" customWidth="1"/>
+    <col min="2" max="9" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="2" spans="1:9">
       <c r="B2" t="s">
         <v>0</v>
@@ -2118,6 +2369,288 @@
       </c>
       <c r="I8">
         <v>51024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>1080071</v>
+      </c>
+      <c r="C14">
+        <v>1016071</v>
+      </c>
+      <c r="D14">
+        <v>326523</v>
+      </c>
+      <c r="E14">
+        <v>278523</v>
+      </c>
+      <c r="F14">
+        <v>327571</v>
+      </c>
+      <c r="G14">
+        <v>263571</v>
+      </c>
+      <c r="H14">
+        <v>114961</v>
+      </c>
+      <c r="I14">
+        <v>66961</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>540039</v>
+      </c>
+      <c r="C15">
+        <v>508039</v>
+      </c>
+      <c r="D15">
+        <v>294523</v>
+      </c>
+      <c r="E15">
+        <v>278523</v>
+      </c>
+      <c r="F15">
+        <v>163789</v>
+      </c>
+      <c r="G15">
+        <v>131789</v>
+      </c>
+      <c r="H15">
+        <v>82961</v>
+      </c>
+      <c r="I15">
+        <v>66961</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>351522</v>
+      </c>
+      <c r="C16">
+        <v>287522</v>
+      </c>
+      <c r="D16">
+        <v>294524</v>
+      </c>
+      <c r="E16">
+        <v>278524</v>
+      </c>
+      <c r="F16">
+        <v>120399</v>
+      </c>
+      <c r="G16">
+        <v>74336</v>
+      </c>
+      <c r="H16">
+        <v>82961</v>
+      </c>
+      <c r="I16">
+        <v>66961</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>251029</v>
+      </c>
+      <c r="C17">
+        <v>235028</v>
+      </c>
+      <c r="D17">
+        <v>294524</v>
+      </c>
+      <c r="E17">
+        <v>278524</v>
+      </c>
+      <c r="F17">
+        <v>100584</v>
+      </c>
+      <c r="G17">
+        <v>74336</v>
+      </c>
+      <c r="H17">
+        <v>82961</v>
+      </c>
+      <c r="I17">
+        <v>66961</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>234529</v>
+      </c>
+      <c r="C18">
+        <v>235028</v>
+      </c>
+      <c r="D18">
+        <v>278024</v>
+      </c>
+      <c r="E18">
+        <v>278524</v>
+      </c>
+      <c r="F18">
+        <v>85647</v>
+      </c>
+      <c r="G18">
+        <v>74336</v>
+      </c>
+      <c r="H18">
+        <v>71961</v>
+      </c>
+      <c r="I18">
+        <v>66961</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>176026</v>
+      </c>
+      <c r="C19">
+        <v>168525</v>
+      </c>
+      <c r="D19">
+        <v>193015</v>
+      </c>
+      <c r="E19">
+        <v>193515</v>
+      </c>
+      <c r="F19">
+        <v>81080</v>
+      </c>
+      <c r="G19">
+        <v>65830</v>
+      </c>
+      <c r="H19">
+        <v>57140</v>
+      </c>
+      <c r="I19">
+        <v>50140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>1080071</v>
+      </c>
+      <c r="C24">
+        <v>340040</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>540039</v>
+      </c>
+      <c r="C25">
+        <v>170022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>351522</v>
+      </c>
+      <c r="C26">
+        <v>139513</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27">
+        <v>251029</v>
+      </c>
+      <c r="C27">
+        <v>66514</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28">
+        <v>234529</v>
+      </c>
+      <c r="C28">
+        <v>42520</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29">
+        <v>176026</v>
+      </c>
+      <c r="C29">
+        <v>42519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>